<commit_message>
update expression adding stanford commencement speech 1
</commit_message>
<xml_diff>
--- a/english_learning/expression.xlsx
+++ b/english_learning/expression.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Having gotten around a bit over the last few years, I am more convinced than ever …</t>
   </si>
@@ -118,9 +118,6 @@
     <t>The joy on his face remains etched in my mind to this day.</t>
   </si>
   <si>
-    <t>But he could well have become one the 9 million children under the age of 5 who die each year, mostly from preventable and treatable afflictions.</t>
-  </si>
-  <si>
     <t>He was perhaps 3 or 4 years old, with pencil-thin legs and a distended belly, and only a torn T-shirt to wear.</t>
   </si>
   <si>
@@ -133,7 +130,46 @@
     <t>…much less served in his cabinet, …</t>
   </si>
   <si>
-    <t>？</t>
+    <t>But he could well have become one of the 9 million children under the age of 5 who die each year, mostly from preventable and treatable afflictions.</t>
+  </si>
+  <si>
+    <t>So we must shape the world that he deserves.</t>
+  </si>
+  <si>
+    <t>Half of humanity lives on less than 2.5 dollars a day.</t>
+  </si>
+  <si>
+    <t>That little boy's future is tied to ours; Our security is ultimately linked to his well-being.</t>
+  </si>
+  <si>
+    <t>That child deserves a world without extreme hunger and dependence that it fosters.</t>
+  </si>
+  <si>
+    <t>Yet Africa's crop production remains the lowest in the world. With your generation's leadership and ingenuity, you can make it the highest.</t>
+  </si>
+  <si>
+    <t>Agricultural research has produced stronger crops that yield more, adapt faster, and better resist drought, disease, and pests.</t>
+  </si>
+  <si>
+    <t>a quality education</t>
+  </si>
+  <si>
+    <t>human trafficking</t>
+  </si>
+  <si>
+    <t>new vaccines for tuberculosis</t>
+  </si>
+  <si>
+    <t>smart therapies that kill cancer cells and leave their healthy neighbors untouched</t>
+  </si>
+  <si>
+    <t>new cures for old plagues</t>
+  </si>
+  <si>
+    <t>needle-free immunizations to stop pandemics in their tracks.</t>
+  </si>
+  <si>
+    <t>They are both children of God, of equal worth, equal consequence, and equal rights.</t>
   </si>
 </sst>
 </file>
@@ -482,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C45"/>
+  <dimension ref="B2:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -516,7 +552,7 @@
         <v>43359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
@@ -524,7 +560,7 @@
         <v>43359</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
@@ -631,7 +667,7 @@
         <v>43359</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
@@ -765,7 +801,7 @@
         <v>43359</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.45">
@@ -813,12 +849,111 @@
         <v>43359</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct some spelling mistakes in expressions.xlsx
</commit_message>
<xml_diff>
--- a/english_learning/expression.xlsx
+++ b/english_learning/expression.xlsx
@@ -208,9 +208,6 @@
     <t>… decided to sample the business world at McKinsey and Company.</t>
   </si>
   <si>
-    <t>… had literally never a spreadsheet.</t>
-  </si>
-  <si>
     <t>I've not followed a pre-ordained path.</t>
   </si>
   <si>
@@ -241,16 +238,19 @@
     <t>struct by serious illnesses</t>
   </si>
   <si>
-    <t>My colleagues were tremendous about stepping in for me at the halls of the United Nations, but nobody could step in forme or for my brother at the hospital.</t>
-  </si>
-  <si>
     <t>a devoted parent</t>
   </si>
   <si>
-    <t>… has a profound responsibility to try with all our skill, all our smrats, and all our soul.</t>
-  </si>
-  <si>
     <t>Congratulations again, and Godspeed.</t>
+  </si>
+  <si>
+    <t>… had literally never met a spreadsheet.</t>
+  </si>
+  <si>
+    <t>My colleagues were tremendous about stepping in for me at the halls of the United Nations, but nobody could step in for me or for my brother at the hospital.</t>
+  </si>
+  <si>
+    <t>… has a profound responsibility to try with all our skill, all our smarts, and all our soul.</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
   <dimension ref="B2:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78:C87"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1138,7 +1138,7 @@
         <v>43362</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.45">
@@ -1146,7 +1146,7 @@
         <v>43362</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.45">
@@ -1154,7 +1154,7 @@
         <v>43362</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.45">
@@ -1162,7 +1162,7 @@
         <v>43362</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.45">
@@ -1170,7 +1170,7 @@
         <v>43362</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.45">
@@ -1178,7 +1178,7 @@
         <v>43363</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.45">
@@ -1186,7 +1186,7 @@
         <v>43363</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.45">
@@ -1194,7 +1194,7 @@
         <v>43363</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.45">
@@ -1202,7 +1202,7 @@
         <v>43363</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.45">
@@ -1210,7 +1210,7 @@
         <v>43363</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.45">
@@ -1218,7 +1218,7 @@
         <v>43363</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.45">
@@ -1226,7 +1226,7 @@
         <v>43363</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.45">
@@ -1234,7 +1234,7 @@
         <v>43363</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.45">
@@ -1242,7 +1242,7 @@
         <v>43363</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.45">
@@ -1250,7 +1250,7 @@
         <v>43363</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>